<commit_message>
Cluster: import wizard with video list
</commit_message>
<xml_diff>
--- a/public/sample/job_cluster.xlsx
+++ b/public/sample/job_cluster.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="cluster" sheetId="1" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <si>
     <t>code</t>
   </si>
@@ -22,6 +22,9 @@
     <t>original_from_vod</t>
   </si>
   <si>
+    <t>video_codes</t>
+  </si>
+  <si>
     <t>cluster_01</t>
   </si>
   <si>
@@ -31,6 +34,9 @@
     <t>១.ផ្នែកកសិកម្ម ស្បៀងអាហារ និងធនធានធម្មជាតិ</t>
   </si>
   <si>
+    <t>vdo_0033;vdo_0035;vdo_0038</t>
+  </si>
+  <si>
     <t>cluster_02</t>
   </si>
   <si>
@@ -40,6 +46,9 @@
     <t>២.ផ្នែកស្ថាបត្យកម្ម និងសំណង់</t>
   </si>
   <si>
+    <t>vdo_0023;vdo_0031;vdo_0043</t>
+  </si>
+  <si>
     <t>cluster_03</t>
   </si>
   <si>
@@ -49,6 +58,9 @@
     <t>៣.ផ្នែកសិល្បៈបច្ចេកវិទ្យា និងសារគមនាគមន៍</t>
   </si>
   <si>
+    <t>vdo_0007;vdo_0011;vdo_0012;vdo_0015;vdo_0019;vdo_0045;vdo_0047;vdo_0049;vdo_0050;vdo_0051</t>
+  </si>
+  <si>
     <t>cluster_04</t>
   </si>
   <si>
@@ -58,6 +70,9 @@
     <t>៤.ផែ្នកសេដ្ឋកិច្ច ពាណិជ្ជកម្ម និងរដ្ឋបាល</t>
   </si>
   <si>
+    <t>vdo_0013;vdo_0017;vdo_0026;vdo_0046</t>
+  </si>
+  <si>
     <t>cluster_05</t>
   </si>
   <si>
@@ -67,6 +82,9 @@
     <t>៥.ផ្នែកអប់រំ និងបណ្តុះបណ្តាល</t>
   </si>
   <si>
+    <t>vdo_0027;vdo_0048;vdo_0052;vdo_0053;vdo_0054;vdo_0055;vdo_0056;vdo_0057;vdo_0058;vdo_0059</t>
+  </si>
+  <si>
     <t>cluster_06</t>
   </si>
   <si>
@@ -76,6 +94,9 @@
     <t>៦.ផ្នែកធនាគារ ហិរញ្ញវត្ថុ និងធានារ៉ាប់រង</t>
   </si>
   <si>
+    <t>vdo_0021;vdo_0030</t>
+  </si>
+  <si>
     <t>cluster_07</t>
   </si>
   <si>
@@ -94,6 +115,9 @@
     <t>៨.ផ្នែកវិទ្យាសាស្រ្តសុខាភិបាល</t>
   </si>
   <si>
+    <t>vdo_0034;vdo_0036;vdo_0037;vdo_0041</t>
+  </si>
+  <si>
     <t>cluster_09</t>
   </si>
   <si>
@@ -103,6 +127,9 @@
     <t>៩.ផ្នែកបដិសណ្ឋារកិច្ច ទេសចរណ៍ និងកម្សាន្ត</t>
   </si>
   <si>
+    <t>vdo_0004;vdo_0024;vdo_0025;vdo_0028</t>
+  </si>
+  <si>
     <t>cluster_10</t>
   </si>
   <si>
@@ -112,6 +139,9 @@
     <t>១០.ផ្នែកសេវាកម្មសាធារណជន</t>
   </si>
   <si>
+    <t>vdo_0009;vdo_0010;vdo_0029;vdo_0039;vdo_0044</t>
+  </si>
+  <si>
     <t>cluster_11</t>
   </si>
   <si>
@@ -121,6 +151,9 @@
     <t>១១.ផ្នែកបច្ចេកវិទ្យាព័ត៌មានវិទ្យា</t>
   </si>
   <si>
+    <t>vdo_0002;vdo_0005;vdo_0006;vdo_0008;vdo_0014;vdo_0022;vdo_0040;vdo_0042</t>
+  </si>
+  <si>
     <t>cluster_12</t>
   </si>
   <si>
@@ -148,6 +181,9 @@
     <t>១៤.ផែ្នកទីផ្សារ និងសេវាកម្មអតិថិជន</t>
   </si>
   <si>
+    <t>vdo_0001;vdo_0003</t>
+  </si>
+  <si>
     <t>cluster_15</t>
   </si>
   <si>
@@ -157,6 +193,9 @@
     <t>១៥.ផ្នែកវិទ្យាសាស្រ្ត បច្ចេកវិទ្យា វិស្វកម្ម និងគណិតសាស្រ្ត</t>
   </si>
   <si>
+    <t>vdo_0016;vdo_0018;vdo_0020</t>
+  </si>
+  <si>
     <t>cluster_16</t>
   </si>
   <si>
@@ -164,6 +203,9 @@
   </si>
   <si>
     <t>១៦.ផ្នែកដឹកជញ្ជូន និងចែកចាយ</t>
+  </si>
+  <si>
+    <t>vdo_0032</t>
   </si>
 </sst>
 </file>
@@ -462,181 +504,223 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>14</v>
+        <v>18</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>17</v>
+        <v>22</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>20</v>
+        <v>26</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>32</v>
+        <v>41</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>35</v>
+        <v>45</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>40</v>
+        <v>51</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>44</v>
+        <v>55</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>47</v>
+        <v>59</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>50</v>
+        <v>63</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>